<commit_message>
set up for free recall sensitivity and specificy
</commit_message>
<xml_diff>
--- a/free_recall_SHINY/Test Data RGN/Huff et al human coded.xlsx
+++ b/free_recall_SHINY/Test Data RGN/Huff et al human coded.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjhuf\OneDrive\Guess-Test Project\GRAM 2016 Blocked vs Single RGN Test\Blocked Tasks Exp A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\lrd\free_recall_SHINY\Test Data RGN\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1348B930-E71D-45C2-B6CD-E384B3E9A989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11835" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="10155" windowHeight="9360" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version A - Guess First" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,22 @@
     <sheet name="Version F - Restudy First" sheetId="6" r:id="rId6"/>
     <sheet name="Data Summary Sheet" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="694">
   <si>
     <t>Subject Number</t>
   </si>
@@ -2105,11 +2116,14 @@
   <si>
     <t>A1F2MFSHXTGAVD</t>
   </si>
+  <si>
+    <t>A1OSRAPSRT9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2303,6 +2317,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2338,6 +2369,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2513,7 +2561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF249"/>
   <sheetViews>
     <sheetView topLeftCell="A217" workbookViewId="0">
@@ -18037,7 +18085,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A25:A29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:A29">
     <sortCondition ref="A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18045,7 +18093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF228"/>
   <sheetViews>
     <sheetView topLeftCell="A194" workbookViewId="0">
@@ -32275,7 +32323,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:A23">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A23">
     <sortCondition ref="A4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32284,7 +32332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG251"/>
   <sheetViews>
     <sheetView topLeftCell="E205" zoomScaleNormal="100" workbookViewId="0">
@@ -48645,7 +48693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE248"/>
   <sheetViews>
     <sheetView topLeftCell="C214" workbookViewId="0">
@@ -63327,7 +63375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE271"/>
   <sheetViews>
     <sheetView topLeftCell="C246" workbookViewId="0">
@@ -79457,7 +79505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AG256"/>
   <sheetViews>
     <sheetView topLeftCell="E223" workbookViewId="0">
@@ -95978,11 +96026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -96018,25 +96066,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>495</v>
+        <v>693</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D2">
         <v>0.32499999999999996</v>
       </c>
       <c r="E2">
-        <v>0.32499999999999996</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="F2">
-        <v>0.35</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -96047,22 +96095,22 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>496</v>
+        <v>419</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="D3">
-        <v>0.52500000000000002</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E3">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="F3">
-        <v>0.3</v>
+        <v>0.375</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -96076,7 +96124,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>316</v>
+        <v>495</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -96088,10 +96136,10 @@
         <v>0.32499999999999996</v>
       </c>
       <c r="E4">
-        <v>0.55000000000000004</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="F4">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -96105,7 +96153,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -96114,13 +96162,13 @@
         <v>686</v>
       </c>
       <c r="D5">
-        <v>0.57499999999999996</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E5">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="F5">
-        <v>0.47499999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -96134,7 +96182,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -96143,13 +96191,13 @@
         <v>686</v>
       </c>
       <c r="D6">
-        <v>0.45</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="E6">
-        <v>0.52500000000000002</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -96163,19 +96211,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>390</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D7">
-        <v>0.42500000000000004</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E7">
-        <v>0.57499999999999996</v>
+        <v>0.45</v>
       </c>
       <c r="F7">
         <v>0.35</v>
@@ -96192,22 +96240,22 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>498</v>
+        <v>635</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="E8">
-        <v>0.42499999999999999</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="F8">
-        <v>0.25</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -96220,87 +96268,87 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>499</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>686</v>
-      </c>
-      <c r="D9">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="E9">
-        <v>0.5</v>
-      </c>
-      <c r="F9">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
+      <c r="A9" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>319</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>686</v>
-      </c>
-      <c r="D10">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E10">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="F10">
-        <v>0.35</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0.1</v>
-      </c>
-      <c r="I10">
+      <c r="A10" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>500</v>
+        <v>636</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="D11">
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0.25</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F11">
-        <v>0.15</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -96308,22 +96356,22 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>593</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="D12">
         <v>0.55000000000000004</v>
       </c>
       <c r="E12">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F12">
         <v>0.45</v>
-      </c>
-      <c r="F12">
-        <v>0.5</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -96337,22 +96385,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>315</v>
+        <v>692</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D13">
+        <v>0.375</v>
+      </c>
+      <c r="E13">
+        <v>0.45</v>
+      </c>
+      <c r="F13">
         <v>0.27500000000000002</v>
-      </c>
-      <c r="E13">
-        <v>0.25</v>
-      </c>
-      <c r="F13">
-        <v>0.2</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -96366,22 +96414,22 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>331</v>
+        <v>565</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D14">
-        <v>0.47500000000000003</v>
+        <v>0.375</v>
       </c>
       <c r="E14">
-        <v>0.47500000000000003</v>
+        <v>0.375</v>
       </c>
       <c r="F14">
-        <v>0.42499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -96394,55 +96442,55 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>502</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>686</v>
-      </c>
-      <c r="D15">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="E15">
-        <v>0.6</v>
-      </c>
-      <c r="F15">
+      <c r="A15" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F15" s="3">
         <v>0.32499999999999996</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>339</v>
+        <v>531</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D16">
-        <v>0.47500000000000003</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="E16">
-        <v>0.625</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="F16">
-        <v>0.42499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -96453,7 +96501,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>344</v>
+        <v>497</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -96462,10 +96510,10 @@
         <v>686</v>
       </c>
       <c r="D17">
-        <v>0.32500000000000001</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="E17">
-        <v>0.47499999999999998</v>
+        <v>0.65</v>
       </c>
       <c r="F17">
         <v>0.47499999999999998</v>
@@ -96482,22 +96530,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>503</v>
+        <v>594</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="D18">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="E18">
-        <v>0.42500000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="F18">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -96510,37 +96558,37 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>345</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>686</v>
-      </c>
-      <c r="D19">
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="E19">
-        <v>0.35</v>
-      </c>
-      <c r="F19">
+      <c r="A19" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F19" s="3">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>504</v>
+        <v>317</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -96549,13 +96597,13 @@
         <v>686</v>
       </c>
       <c r="D20">
-        <v>0.75</v>
+        <v>0.45</v>
       </c>
       <c r="E20">
-        <v>0.64999999999999991</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F20">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -96569,181 +96617,181 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>346</v>
+        <v>566</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D21">
-        <v>0.44999999999999996</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="E21">
-        <v>0.42500000000000004</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F21">
+        <v>0.3</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>637</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>691</v>
+      </c>
+      <c r="D22">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="E22">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F22">
+        <v>0.35</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>367</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>688</v>
+      </c>
+      <c r="D23">
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="E23">
+        <v>0.3</v>
+      </c>
+      <c r="F23">
+        <v>0.35</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>420</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>690</v>
+      </c>
+      <c r="D24">
+        <v>0.6</v>
+      </c>
+      <c r="E24">
+        <v>0.65</v>
+      </c>
+      <c r="F24">
+        <v>0.5</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>532</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>688</v>
+      </c>
+      <c r="D25">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>421</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>690</v>
+      </c>
+      <c r="D26">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E26">
         <v>0.375</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.47500000000000003</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.52499999999999991</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="F26">
+        <v>0.25</v>
+      </c>
+      <c r="G26">
+        <v>0.2</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>513</v>
+        <v>466</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -96752,451 +96800,451 @@
         <v>687</v>
       </c>
       <c r="D27" s="3">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>394</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>689</v>
+      </c>
+      <c r="D28">
+        <v>0.25</v>
+      </c>
+      <c r="E28">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>318</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>686</v>
+      </c>
+      <c r="D29">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="E29">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F29">
+        <v>0.35</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>498</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>686</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="F30">
+        <v>0.25</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>422</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>690</v>
+      </c>
+      <c r="D31">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E31">
+        <v>0.65</v>
+      </c>
+      <c r="F31">
+        <v>0.45</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>691</v>
+      </c>
+      <c r="D32">
+        <v>0.45</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <v>0.35</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>449</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>691</v>
+      </c>
+      <c r="D33">
         <v>0.4</v>
       </c>
-      <c r="E27" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="F27" s="3">
+      <c r="E33">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F33">
+        <v>0.2</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>595</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>690</v>
+      </c>
+      <c r="D34">
+        <v>0.35</v>
+      </c>
+      <c r="E34">
+        <v>0.35</v>
+      </c>
+      <c r="F34">
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>370</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>688</v>
+      </c>
+      <c r="D35">
+        <v>0.1</v>
+      </c>
+      <c r="E35">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="F35">
+        <v>0.1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>596</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>690</v>
+      </c>
+      <c r="D36">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="E36">
+        <v>0.8</v>
+      </c>
+      <c r="F36">
+        <v>0.5</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>499</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>686</v>
+      </c>
+      <c r="D37">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="E37">
+        <v>0.5</v>
+      </c>
+      <c r="F37">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>597</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>690</v>
+      </c>
+      <c r="D38">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="E38">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="F38">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>598</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>690</v>
+      </c>
+      <c r="D39">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E39">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F39">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>533</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>688</v>
+      </c>
+      <c r="D40">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E40">
         <v>0.45</v>
       </c>
-      <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.42500000000000004</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="F40">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>567</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>689</v>
+      </c>
+      <c r="D41">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E41">
         <v>0.45</v>
       </c>
-      <c r="F29" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F30" s="3">
+      <c r="F41">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G30" s="3">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0.72500000000000009</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0</v>
-      </c>
-      <c r="H31" s="3">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.47500000000000003</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I35" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0</v>
-      </c>
-      <c r="H36" s="3">
-        <v>0</v>
-      </c>
-      <c r="I36" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G37" s="3">
-        <v>0</v>
-      </c>
-      <c r="H37" s="3">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="E38" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0</v>
-      </c>
-      <c r="H38" s="3">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="E39" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0</v>
-      </c>
-      <c r="H39" s="3">
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D41" s="3">
-        <v>0.42500000000000004</v>
-      </c>
-      <c r="E41" s="3">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G41" s="3">
-        <v>0</v>
-      </c>
-      <c r="H41" s="3">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>365</v>
+        <v>423</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D42">
-        <v>0.32499999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="E42">
-        <v>0.22500000000000001</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F42">
-        <v>0.22499999999999998</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="G42">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -97207,7 +97255,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -97216,16 +97264,16 @@
         <v>688</v>
       </c>
       <c r="D43">
+        <v>0.35</v>
+      </c>
+      <c r="E43">
+        <v>0.4</v>
+      </c>
+      <c r="F43">
         <v>0.27500000000000002</v>
       </c>
-      <c r="E43">
-        <v>0.42500000000000004</v>
-      </c>
-      <c r="F43">
-        <v>0.25</v>
-      </c>
       <c r="G43">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -97236,19 +97284,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D44">
-        <v>0.32499999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E44">
-        <v>0.3</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F44">
         <v>0.35</v>
@@ -97257,7 +97305,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -97265,28 +97313,28 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>532</v>
+        <v>500</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D45">
-        <v>0.47499999999999998</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="E45">
-        <v>0.55000000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="F45">
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -97294,83 +97342,83 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>370</v>
+        <v>568</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D46">
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="E46">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F46">
+        <v>0.3</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <v>0.1</v>
       </c>
-      <c r="E46">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="F46">
-        <v>0.1</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
       <c r="I46">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>533</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>688</v>
-      </c>
-      <c r="D47">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="E47">
+      <c r="A47" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F47" s="3">
         <v>0.45</v>
       </c>
-      <c r="F47">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>534</v>
+        <v>395</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D48">
-        <v>0.35</v>
+        <v>0.6</v>
       </c>
       <c r="E48">
-        <v>0.4</v>
+        <v>0.625</v>
       </c>
       <c r="F48">
-        <v>0.27500000000000002</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G48">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -97381,80 +97429,80 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>535</v>
+        <v>450</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="D49">
-        <v>0.47499999999999998</v>
+        <v>0.8</v>
       </c>
       <c r="E49">
-        <v>0.45</v>
+        <v>0.875</v>
       </c>
       <c r="F49">
+        <v>0.875</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F50" s="3">
         <v>0.375</v>
       </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>377</v>
-      </c>
-      <c r="B50">
-        <v>2</v>
-      </c>
-      <c r="C50" t="s">
-        <v>688</v>
-      </c>
-      <c r="D50">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="E50">
-        <v>0.7</v>
-      </c>
-      <c r="F50">
-        <v>0.75</v>
-      </c>
-      <c r="G50">
-        <v>0.2</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>536</v>
+        <v>638</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="D51">
-        <v>0.60000000000000009</v>
+        <v>0.45</v>
       </c>
       <c r="E51">
-        <v>0.57499999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="F51">
-        <v>0.57499999999999996</v>
+        <v>0.35</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -97468,22 +97516,22 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D52">
-        <v>0.6</v>
+        <v>0.625</v>
       </c>
       <c r="E52">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="F52">
-        <v>0.55000000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -97496,52 +97544,52 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>537</v>
-      </c>
-      <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="C53" t="s">
-        <v>688</v>
-      </c>
-      <c r="D53">
-        <v>0.35</v>
-      </c>
-      <c r="E53">
-        <v>0.35</v>
-      </c>
-      <c r="F53">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
+      <c r="A53" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>380</v>
+        <v>501</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D54">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E54">
         <v>0.45</v>
       </c>
-      <c r="E54">
-        <v>0.72499999999999998</v>
-      </c>
       <c r="F54">
-        <v>0.42500000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -97555,22 +97603,22 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>386</v>
+        <v>315</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D55">
-        <v>0.5</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="E55">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F55">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -97584,22 +97632,22 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>387</v>
+        <v>639</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="D56">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E56">
         <v>0.57499999999999996</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>0.375</v>
-      </c>
-      <c r="F56">
-        <v>0.52500000000000002</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -97613,25 +97661,25 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>388</v>
+        <v>331</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D57">
-        <v>0.47499999999999998</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="E57">
-        <v>0.375</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="F57">
-        <v>0.52500000000000002</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="G57">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -97642,7 +97690,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -97654,10 +97702,10 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="E58">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="F58">
-        <v>0.55000000000000004</v>
+        <v>0.375</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -97671,7 +97719,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>539</v>
+        <v>377</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -97680,16 +97728,16 @@
         <v>688</v>
       </c>
       <c r="D59">
-        <v>0.31052631578947365</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E59">
-        <v>0.47499999999999998</v>
+        <v>0.7</v>
       </c>
       <c r="F59">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -97700,25 +97748,25 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>540</v>
+        <v>569</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D60">
-        <v>0.47499999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="E60">
-        <v>0.5</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F60">
-        <v>0.625</v>
+        <v>0.56447368421052635</v>
       </c>
       <c r="G60">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -97729,7 +97777,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -97738,13 +97786,13 @@
         <v>688</v>
       </c>
       <c r="D61">
-        <v>0.42500000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="E61">
-        <v>0.2</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="F61">
-        <v>0.17499999999999999</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -97758,80 +97806,80 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>389</v>
+        <v>570</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D62">
-        <v>0.55000000000000004</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="E62">
+        <v>0.2</v>
+      </c>
+      <c r="F62">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="E63" s="3">
         <v>0.57499999999999996</v>
       </c>
-      <c r="F62">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>390</v>
-      </c>
-      <c r="B63">
-        <v>2</v>
-      </c>
-      <c r="C63" t="s">
-        <v>689</v>
-      </c>
-      <c r="D63">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E63">
-        <v>0.45</v>
-      </c>
-      <c r="F63">
-        <v>0.35</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
+      <c r="F63" s="3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G63" s="3">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>565</v>
+        <v>462</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D64">
-        <v>0.375</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E64">
-        <v>0.375</v>
+        <v>0.6</v>
       </c>
       <c r="F64">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -97845,22 +97893,22 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>692</v>
+        <v>502</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D65">
-        <v>0.375</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E65">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="F65">
-        <v>0.27500000000000002</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -97874,25 +97922,25 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>566</v>
+        <v>640</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D66">
-        <v>0.42499999999999999</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E66">
-        <v>0.52500000000000002</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="F66">
-        <v>0.3</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G66">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -97903,22 +97951,22 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>394</v>
+        <v>339</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D67">
-        <v>0.25</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="E67">
-        <v>0.22499999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="F67">
-        <v>0.22500000000000001</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -97932,77 +97980,77 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>567</v>
+        <v>344</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D68">
-        <v>0.55000000000000004</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="E68">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F68">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E69" s="3">
+        <v>0.72500000000000009</v>
+      </c>
+      <c r="F69" s="3">
         <v>0.45</v>
       </c>
-      <c r="F68">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>568</v>
-      </c>
-      <c r="B69">
-        <v>2</v>
-      </c>
-      <c r="C69" t="s">
-        <v>689</v>
-      </c>
-      <c r="D69">
-        <v>0.52499999999999991</v>
-      </c>
-      <c r="E69">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="F69">
-        <v>0.3</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0.1</v>
-      </c>
-      <c r="I69">
+      <c r="G69" s="3">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="B70">
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D70">
         <v>0.6</v>
       </c>
       <c r="E70">
-        <v>0.625</v>
+        <v>0.65</v>
       </c>
       <c r="F70">
         <v>0.55000000000000004</v>
@@ -98019,22 +98067,22 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>397</v>
+        <v>537</v>
       </c>
       <c r="B71">
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D71">
-        <v>0.625</v>
+        <v>0.35</v>
       </c>
       <c r="E71">
-        <v>0.75</v>
+        <v>0.35</v>
       </c>
       <c r="F71">
-        <v>0.75</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -98048,7 +98096,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -98057,19 +98105,19 @@
         <v>689</v>
       </c>
       <c r="D72">
-        <v>0.6</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="E72">
-        <v>0.60000000000000009</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F72">
-        <v>0.56447368421052635</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -98077,7 +98125,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -98086,13 +98134,13 @@
         <v>689</v>
       </c>
       <c r="D73">
-        <v>0.27500000000000002</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="E73">
-        <v>0.2</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F73">
-        <v>0.22499999999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -98106,28 +98154,28 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>571</v>
+        <v>438</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D74">
-        <v>0.57499999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="E74">
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="F74">
-        <v>0.32500000000000001</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G74">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -98135,22 +98183,22 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>572</v>
+        <v>599</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D75">
-        <v>0.47500000000000003</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E75">
-        <v>0.47499999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="F75">
-        <v>0.47499999999999998</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -98164,22 +98212,22 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>573</v>
+        <v>380</v>
       </c>
       <c r="B76">
         <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D76">
-        <v>0.60000000000000009</v>
+        <v>0.45</v>
       </c>
       <c r="E76">
-        <v>0.47499999999999998</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="F76">
-        <v>0.47499999999999998</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -98193,22 +98241,22 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>398</v>
+        <v>458</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D77">
-        <v>0.75</v>
+        <v>0.3</v>
       </c>
       <c r="E77">
-        <v>0.67500000000000004</v>
+        <v>0.375</v>
       </c>
       <c r="F77">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -98222,22 +98270,22 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>399</v>
+        <v>503</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D78">
-        <v>0.55000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="E78">
-        <v>0.47499999999999998</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="F78">
-        <v>0.52500000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -98251,22 +98299,22 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>400</v>
+        <v>641</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D79">
-        <v>0.42500000000000004</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="E79">
-        <v>0.27500000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="F79">
-        <v>0.27500000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -98280,16 +98328,16 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>401</v>
+        <v>642</v>
       </c>
       <c r="B80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D80">
-        <v>0.42500000000000004</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="E80">
         <v>0.42500000000000004</v>
@@ -98309,22 +98357,22 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="B81">
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D81">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E81">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F81">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -98337,37 +98385,37 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>419</v>
-      </c>
-      <c r="B82">
-        <v>3</v>
-      </c>
-      <c r="C82" t="s">
-        <v>690</v>
-      </c>
-      <c r="D82">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="E82">
-        <v>0.45</v>
-      </c>
-      <c r="F82">
-        <v>0.375</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82">
+      <c r="A82" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D82" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="G82" s="3">
+        <v>0</v>
+      </c>
+      <c r="H82" s="3">
+        <v>0</v>
+      </c>
+      <c r="I82" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -98376,13 +98424,13 @@
         <v>690</v>
       </c>
       <c r="D83">
-        <v>0.55000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="E83">
         <v>0.52500000000000002</v>
       </c>
       <c r="F83">
-        <v>0.45</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -98395,84 +98443,84 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>594</v>
-      </c>
-      <c r="B84">
-        <v>3</v>
-      </c>
-      <c r="C84" t="s">
-        <v>690</v>
-      </c>
-      <c r="D84">
-        <v>0.4</v>
-      </c>
-      <c r="E84">
-        <v>0.45</v>
-      </c>
-      <c r="F84">
-        <v>0.45</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84">
+      <c r="A84" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D84" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E84" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="F84" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="G84" s="3">
+        <v>0</v>
+      </c>
+      <c r="H84" s="3">
+        <v>0</v>
+      </c>
+      <c r="I84" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>420</v>
-      </c>
-      <c r="B85">
-        <v>3</v>
-      </c>
-      <c r="C85" t="s">
-        <v>690</v>
-      </c>
-      <c r="D85">
-        <v>0.6</v>
-      </c>
-      <c r="E85">
-        <v>0.65</v>
-      </c>
-      <c r="F85">
-        <v>0.5</v>
-      </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85">
+      <c r="A85" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D85" s="3">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="E85" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G85" s="3">
+        <v>0</v>
+      </c>
+      <c r="H85" s="3">
+        <v>0</v>
+      </c>
+      <c r="I85" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D86">
-        <v>0.42499999999999999</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="E86">
-        <v>0.375</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F86">
-        <v>0.25</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="G86">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -98483,22 +98531,22 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>422</v>
+        <v>387</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D87">
-        <v>0.67500000000000004</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="E87">
-        <v>0.65</v>
+        <v>0.375</v>
       </c>
       <c r="F87">
-        <v>0.45</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -98512,22 +98560,22 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>595</v>
+        <v>398</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D88">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="E88">
-        <v>0.35</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F88">
-        <v>0.32499999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -98540,52 +98588,52 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>596</v>
-      </c>
-      <c r="B89">
-        <v>3</v>
-      </c>
-      <c r="C89" t="s">
-        <v>690</v>
-      </c>
-      <c r="D89">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="E89">
-        <v>0.8</v>
-      </c>
-      <c r="F89">
-        <v>0.5</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89">
+      <c r="A89" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D89" s="3">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E89" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G89" s="3">
+        <v>0</v>
+      </c>
+      <c r="H89" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I89" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>597</v>
+        <v>399</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D90">
-        <v>0.22499999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E90">
-        <v>0.17499999999999999</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F90">
-        <v>0.17499999999999999</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -98598,52 +98646,52 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>598</v>
-      </c>
-      <c r="B91">
-        <v>3</v>
-      </c>
-      <c r="C91" t="s">
-        <v>690</v>
-      </c>
-      <c r="D91">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="E91">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F91">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91">
+      <c r="A91" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D91" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E91" s="3">
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G91" s="3">
+        <v>0</v>
+      </c>
+      <c r="H91" s="3">
+        <v>0</v>
+      </c>
+      <c r="I91" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>423</v>
+        <v>643</v>
       </c>
       <c r="B92">
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D92">
-        <v>0.4</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="E92">
-        <v>0.47499999999999998</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="F92">
-        <v>0.47500000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -98657,25 +98705,25 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>438</v>
+        <v>388</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D93">
-        <v>0.4</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E93">
-        <v>0.4</v>
+        <v>0.375</v>
       </c>
       <c r="F93">
-        <v>0.27500000000000002</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -98686,22 +98734,22 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>599</v>
+        <v>345</v>
       </c>
       <c r="B94">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="D94">
-        <v>0.55000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="E94">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="F94">
-        <v>0.32500000000000001</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -98715,22 +98763,22 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="B95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D95">
-        <v>0.35</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="E95">
-        <v>0.52500000000000002</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F95">
-        <v>0.57499999999999996</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -98744,25 +98792,25 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>439</v>
+        <v>459</v>
       </c>
       <c r="B96">
         <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D96">
         <v>0.42500000000000004</v>
       </c>
       <c r="E96">
-        <v>0.52500000000000002</v>
+        <v>0.45</v>
       </c>
       <c r="F96">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="G96">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -98773,22 +98821,22 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>440</v>
+        <v>644</v>
       </c>
       <c r="B97">
         <v>3</v>
       </c>
       <c r="C97" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D97">
-        <v>0.875</v>
+        <v>0.65</v>
       </c>
       <c r="E97">
-        <v>0.9</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="F97">
-        <v>0.57499999999999996</v>
+        <v>0.35</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -98801,52 +98849,52 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>441</v>
-      </c>
-      <c r="B98">
-        <v>3</v>
-      </c>
-      <c r="C98" t="s">
-        <v>690</v>
-      </c>
-      <c r="D98">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="E98">
-        <v>0.72500000000000009</v>
-      </c>
-      <c r="F98">
-        <v>0.35</v>
-      </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
-      <c r="I98">
+      <c r="A98" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B98" s="3">
+        <v>1</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D98" s="3">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E98" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G98" s="3">
+        <v>0</v>
+      </c>
+      <c r="H98" s="3">
+        <v>0</v>
+      </c>
+      <c r="I98" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="B99">
         <v>3</v>
       </c>
       <c r="C99" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D99">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="E99">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="F99">
-        <v>0.875</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -98860,22 +98908,22 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>601</v>
+        <v>401</v>
       </c>
       <c r="B100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D100">
-        <v>0.75</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="E100">
-        <v>0.47500000000000003</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="F100">
-        <v>0.375</v>
+        <v>0.2</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -98889,22 +98937,22 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>635</v>
+        <v>402</v>
       </c>
       <c r="B101">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D101">
         <v>0.45</v>
       </c>
       <c r="E101">
-        <v>0.32500000000000001</v>
+        <v>0.375</v>
       </c>
       <c r="F101">
-        <v>0.27500000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -98918,7 +98966,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>636</v>
+        <v>461</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -98927,13 +98975,13 @@
         <v>691</v>
       </c>
       <c r="D102">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="E102">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="F102">
         <v>0.5</v>
-      </c>
-      <c r="E102">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F102">
-        <v>0.27500000000000002</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -98947,22 +98995,22 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>637</v>
+        <v>504</v>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D103">
-        <v>0.47500000000000003</v>
+        <v>0.75</v>
       </c>
       <c r="E103">
-        <v>0.52500000000000002</v>
+        <v>0.64999999999999991</v>
       </c>
       <c r="F103">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -98976,22 +99024,22 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>448</v>
+        <v>346</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D104">
-        <v>0.45</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="E104">
-        <v>0.5</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="F104">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -99005,25 +99053,25 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D105">
-        <v>0.4</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="E105">
-        <v>0.60000000000000009</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F105">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -99034,22 +99082,22 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="B106">
         <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D106">
-        <v>0.8</v>
+        <v>0.875</v>
       </c>
       <c r="E106">
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="F106">
-        <v>0.875</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -99062,52 +99110,52 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>638</v>
-      </c>
-      <c r="B107">
-        <v>3</v>
-      </c>
-      <c r="C107" t="s">
-        <v>691</v>
-      </c>
-      <c r="D107">
+      <c r="A107" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B107" s="3">
+        <v>1</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D107" s="3">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E107" s="3">
         <v>0.45</v>
       </c>
-      <c r="E107">
-        <v>0.5</v>
-      </c>
-      <c r="F107">
-        <v>0.35</v>
-      </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107">
-        <v>0</v>
-      </c>
-      <c r="I107">
+      <c r="F107" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G107" s="3">
+        <v>0</v>
+      </c>
+      <c r="H107" s="3">
+        <v>0</v>
+      </c>
+      <c r="I107" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>639</v>
+        <v>538</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D108">
-        <v>0.60000000000000009</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E108">
-        <v>0.57499999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="F108">
-        <v>0.375</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -99121,7 +99169,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="B109">
         <v>3</v>
@@ -99130,13 +99178,13 @@
         <v>691</v>
       </c>
       <c r="D109">
-        <v>0.55000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="E109">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="F109">
-        <v>0.125</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -99149,37 +99197,37 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>640</v>
-      </c>
-      <c r="B110">
-        <v>3</v>
-      </c>
-      <c r="C110" t="s">
-        <v>691</v>
-      </c>
-      <c r="D110">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="E110">
-        <v>0.42500000000000004</v>
-      </c>
-      <c r="F110">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110">
+      <c r="A110" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B110" s="3">
+        <v>1</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D110" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="E110" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F110" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="G110" s="3">
+        <v>0</v>
+      </c>
+      <c r="H110" s="3">
+        <v>0</v>
+      </c>
+      <c r="I110" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>458</v>
+        <v>494</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -99188,16 +99236,16 @@
         <v>691</v>
       </c>
       <c r="D111">
-        <v>0.3</v>
+        <v>0.375</v>
       </c>
       <c r="E111">
-        <v>0.375</v>
+        <v>0.45</v>
       </c>
       <c r="F111">
-        <v>0.2</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -99208,22 +99256,22 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>641</v>
+        <v>539</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D112">
-        <v>0.17499999999999999</v>
+        <v>0.31052631578947365</v>
       </c>
       <c r="E112">
-        <v>0.15</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F112">
-        <v>0.05</v>
+        <v>0.45</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -99237,25 +99285,25 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>642</v>
+        <v>540</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D113">
-        <v>0.32500000000000001</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E113">
-        <v>0.42500000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F113">
-        <v>0.2</v>
+        <v>0.625</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -99266,22 +99314,22 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>643</v>
+        <v>541</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D114">
         <v>0.42500000000000004</v>
       </c>
       <c r="E114">
-        <v>0.32499999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="F114">
-        <v>0.25</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -99295,7 +99343,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>459</v>
+        <v>645</v>
       </c>
       <c r="B115">
         <v>3</v>
@@ -99304,16 +99352,16 @@
         <v>691</v>
       </c>
       <c r="D115">
-        <v>0.42500000000000004</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E115">
-        <v>0.45</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F115">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H115">
         <v>0</v>
@@ -99324,19 +99372,19 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>644</v>
+        <v>441</v>
       </c>
       <c r="B116">
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D116">
-        <v>0.65</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E116">
-        <v>0.32500000000000001</v>
+        <v>0.72500000000000009</v>
       </c>
       <c r="F116">
         <v>0.35</v>
@@ -99353,22 +99401,22 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B117">
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D117">
-        <v>0.45</v>
+        <v>0.65</v>
       </c>
       <c r="E117">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="F117">
-        <v>0.47499999999999998</v>
+        <v>0.875</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -99382,22 +99430,22 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>461</v>
+        <v>601</v>
       </c>
       <c r="B118">
         <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D118">
-        <v>0.42500000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="E118">
         <v>0.47500000000000003</v>
       </c>
       <c r="F118">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -99411,22 +99459,22 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>476</v>
+        <v>389</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D119">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E119">
-        <v>0.25</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="F119">
-        <v>0.19999999999999998</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -99439,66 +99487,66 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>494</v>
-      </c>
-      <c r="B120">
-        <v>3</v>
-      </c>
-      <c r="C120" t="s">
-        <v>691</v>
-      </c>
-      <c r="D120">
-        <v>0.375</v>
-      </c>
-      <c r="E120">
-        <v>0.45</v>
-      </c>
-      <c r="F120">
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="G120">
-        <v>0.1</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-      <c r="I120">
+      <c r="A120" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B120" s="3">
+        <v>1</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D120" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="E120" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="F120" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G120" s="3">
+        <v>0</v>
+      </c>
+      <c r="H120" s="3">
+        <v>0</v>
+      </c>
+      <c r="I120" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>645</v>
-      </c>
-      <c r="B121">
-        <v>3</v>
-      </c>
-      <c r="C121" t="s">
-        <v>691</v>
-      </c>
-      <c r="D121">
+      <c r="A121" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B121" s="3">
+        <v>1</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D121" s="3">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="E121" s="3">
         <v>0.52500000000000002</v>
       </c>
-      <c r="E121">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="F121">
-        <v>0.375</v>
-      </c>
-      <c r="G121">
-        <v>0.1</v>
-      </c>
-      <c r="H121">
-        <v>0</v>
-      </c>
-      <c r="I121">
+      <c r="F121" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G121" s="3">
+        <v>0</v>
+      </c>
+      <c r="H121" s="3">
+        <v>0</v>
+      </c>
+      <c r="I121" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A100:I120">
-    <sortCondition ref="A100:A120"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I121">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ad_hoc sensitivity and specificity
</commit_message>
<xml_diff>
--- a/free_recall_SHINY/Test Data RGN/Huff et al human coded.xlsx
+++ b/free_recall_SHINY/Test Data RGN/Huff et al human coded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\lrd\free_recall_SHINY\Test Data RGN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1348B930-E71D-45C2-B6CD-E384B3E9A989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24806225-5D5D-4CE1-A4DE-E1673D5EA262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="10155" windowHeight="9360" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13680" yWindow="2685" windowWidth="10155" windowHeight="9360" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version A - Guess First" sheetId="1" r:id="rId1"/>
@@ -96030,7 +96030,7 @@
   <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -96066,25 +96066,25 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>693</v>
+        <v>419</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D2">
-        <v>0.32499999999999996</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E2">
-        <v>0.22500000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="F2">
-        <v>0.22499999999999998</v>
+        <v>0.375</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -96095,22 +96095,22 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>419</v>
+        <v>495</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="D3">
-        <v>0.47499999999999998</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="E3">
-        <v>0.45</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="F3">
-        <v>0.375</v>
+        <v>0.35</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -96124,7 +96124,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -96133,13 +96133,13 @@
         <v>686</v>
       </c>
       <c r="D4">
-        <v>0.32499999999999996</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E4">
-        <v>0.32499999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="F4">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -96153,7 +96153,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>496</v>
+        <v>316</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -96162,13 +96162,13 @@
         <v>686</v>
       </c>
       <c r="D5">
-        <v>0.52500000000000002</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="E5">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -96182,22 +96182,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>390</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D6">
-        <v>0.32499999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E6">
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="F6">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -96211,65 +96211,65 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>390</v>
+        <v>635</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D7">
+        <v>0.45</v>
+      </c>
+      <c r="E7">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D8" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E7">
+      <c r="E8" s="3">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="F8" s="3">
         <v>0.45</v>
       </c>
-      <c r="F7">
-        <v>0.35</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>635</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>691</v>
-      </c>
-      <c r="D8">
-        <v>0.45</v>
-      </c>
-      <c r="E8">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="F8">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>512</v>
+        <v>347</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -96278,71 +96278,71 @@
         <v>687</v>
       </c>
       <c r="D9" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>636</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>691</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E9" s="3">
-        <v>0.47500000000000003</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="F10">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>636</v>
+        <v>593</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E11">
-        <v>0.55000000000000004</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F11">
-        <v>0.27500000000000002</v>
+        <v>0.45</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -96356,22 +96356,22 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>593</v>
+        <v>692</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D12">
-        <v>0.55000000000000004</v>
+        <v>0.375</v>
       </c>
       <c r="E12">
-        <v>0.52500000000000002</v>
+        <v>0.45</v>
       </c>
       <c r="F12">
-        <v>0.45</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -96385,7 +96385,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>692</v>
+        <v>565</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -96397,100 +96397,100 @@
         <v>0.375</v>
       </c>
       <c r="E13">
-        <v>0.45</v>
+        <v>0.375</v>
       </c>
       <c r="F13">
+        <v>0.25</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>531</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>688</v>
+      </c>
+      <c r="D15">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>565</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>689</v>
-      </c>
-      <c r="D14">
-        <v>0.375</v>
-      </c>
-      <c r="E14">
-        <v>0.375</v>
-      </c>
-      <c r="F14">
+      <c r="E15">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="F15">
         <v>0.25</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>531</v>
+        <v>497</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D16">
-        <v>0.27500000000000002</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="E16">
-        <v>0.42500000000000004</v>
+        <v>0.65</v>
       </c>
       <c r="F16">
-        <v>0.25</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="G16">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -96501,112 +96501,112 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>497</v>
+        <v>594</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>690</v>
+      </c>
+      <c r="D17">
+        <v>0.4</v>
+      </c>
+      <c r="E17">
+        <v>0.45</v>
+      </c>
+      <c r="F17">
+        <v>0.45</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>686</v>
       </c>
-      <c r="D17">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="E17">
-        <v>0.65</v>
-      </c>
-      <c r="F17">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>594</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>690</v>
-      </c>
-      <c r="D18">
-        <v>0.4</v>
-      </c>
-      <c r="E18">
+      <c r="D19">
         <v>0.45</v>
       </c>
-      <c r="F18">
-        <v>0.45</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.52499999999999991</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="E19">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>317</v>
+        <v>566</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D20">
-        <v>0.45</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="E20">
         <v>0.52500000000000002</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -96617,25 +96617,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>566</v>
+        <v>637</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D21">
-        <v>0.42499999999999999</v>
+        <v>0.47500000000000003</v>
       </c>
       <c r="E21">
         <v>0.52500000000000002</v>
       </c>
       <c r="F21">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="G21">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -96646,25 +96646,25 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>637</v>
+        <v>693</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D22">
-        <v>0.47500000000000003</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="E22">
-        <v>0.52500000000000002</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="F22">
-        <v>0.35</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H22">
         <v>0</v>

</xml_diff>